<commit_message>
Instance variables moved to the top of pages
</commit_message>
<xml_diff>
--- a/MarsCompetition/MarsCompetition/ManageListings.xlsx
+++ b/MarsCompetition/MarsCompetition/ManageListings.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mars\MarsCompetition\MarsCompetition\MarsCompetition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mars\Competition\MarsCompetition\MarsCompetition\MarsCompetition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA6B0DA-0605-48F0-B294-78CBBFB2B5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2323CB57-1DF8-4BC4-9ACC-C28FC845CEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="195" windowWidth="15315" windowHeight="7890" activeTab="2" xr2:uid="{95F67D77-5BEE-421A-9604-670782050B9D}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{95F67D77-5BEE-421A-9604-670782050B9D}"/>
   </bookViews>
   <sheets>
-    <sheet name="JoinPage" sheetId="6" r:id="rId1"/>
-    <sheet name="LoginPage" sheetId="7" r:id="rId2"/>
-    <sheet name="ManageListingsPage" sheetId="8" r:id="rId3"/>
+    <sheet name="ManageListingsPage" sheetId="8" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,40 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="118">
-  <si>
-    <t>http://localhost:5000</t>
-  </si>
-  <si>
-    <t>kgbandula@gmail.com</t>
-  </si>
-  <si>
-    <t>bandula1975</t>
-  </si>
-  <si>
-    <t>Bandula</t>
-  </si>
-  <si>
-    <t>Wimalasena</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>EmailAddress</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ConfirmPassword</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="107">
   <si>
     <t>Title</t>
   </si>
@@ -398,18 +363,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -446,21 +403,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -772,111 +726,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E329CE-1350-4D68-9499-7BA907E1411C}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{B7E16073-E439-43B3-8EE9-C6ABC9F73793}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{46CEB1B4-C217-4566-9E0F-C09BB82B2C2C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65BBC4D-2813-4AEE-AE7A-DF9E2308BB17}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B4B9DE6D-F0F4-41CD-9F0A-99F6ACCF2EB6}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE44C8B-E3EB-49EF-9C06-BCA64E46D57E}">
   <dimension ref="A1:AK8"/>
   <sheetViews>
@@ -919,522 +768,522 @@
     <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="2" t="s">
+    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AF1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>107</v>
+      <c r="AG1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
       <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
         <v>46</v>
       </c>
-      <c r="O2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>57</v>
-      </c>
       <c r="R2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="T2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="U2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="V2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" t="s">
         <v>46</v>
       </c>
-      <c r="W2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>57</v>
-      </c>
       <c r="Z2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="AA2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="AB2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC2" s="3">
+        <v>79</v>
+      </c>
+      <c r="AC2" s="2">
         <v>45137</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AD2" s="2">
         <v>45158</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH2" t="s">
         <v>92</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>103</v>
       </c>
       <c r="AI2">
         <v>4</v>
       </c>
       <c r="AJ2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="AK2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" t="s">
         <v>47</v>
       </c>
-      <c r="O3" t="s">
-        <v>51</v>
-      </c>
-      <c r="P3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>58</v>
-      </c>
       <c r="R3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="S3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="T3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="U3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="V3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" t="s">
         <v>47</v>
       </c>
-      <c r="W3" t="s">
-        <v>51</v>
-      </c>
-      <c r="X3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>58</v>
-      </c>
       <c r="Z3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="AA3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="AB3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC3" s="3">
+        <v>80</v>
+      </c>
+      <c r="AC3" s="2">
         <v>45169</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AD3" s="2">
         <v>45190</v>
       </c>
-      <c r="AE3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>111</v>
+      <c r="AE3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="AH3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="AK3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" t="s">
         <v>48</v>
       </c>
-      <c r="O4" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>59</v>
-      </c>
       <c r="R4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="S4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="T4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="U4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="V4" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y4" t="s">
         <v>48</v>
       </c>
-      <c r="W4" t="s">
-        <v>52</v>
-      </c>
-      <c r="X4" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>59</v>
-      </c>
       <c r="Z4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>112</v>
+        <v>53</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" t="s">
         <v>49</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y5" t="s">
         <v>49</v>
       </c>
-      <c r="P5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5" t="s">
-        <v>65</v>
-      </c>
-      <c r="S5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5" t="s">
-        <v>49</v>
-      </c>
-      <c r="W5" t="s">
-        <v>49</v>
-      </c>
-      <c r="X5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>60</v>
-      </c>
       <c r="Z5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>113</v>
+        <v>54</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="K6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="P6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="R6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="S6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="T6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="U6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="X6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="Y6" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="Z6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF6" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>114</v>
+        <v>55</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="P7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="Q7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="R7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="X7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="Y7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="Z7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF7" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG7" s="4" t="s">
-        <v>115</v>
+        <v>38</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="AE8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF8" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG8" s="4" t="s">
-        <v>116</v>
+      <c r="AE8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>